<commit_message>
Testing core matrix row and column activation
Row 0 has loose connection. Row 1 works in columns 0-3. Row 2 work entirely. Column 0-3 work. Column 4-7 only works for CLEAR, but SET does not show current flow.
</commit_message>
<xml_diff>
--- a/Electronic Design/core flip sense voltage threshold.xlsx
+++ b/Electronic Design/core flip sense voltage threshold.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{7894EA0F-3342-2140-B87D-CBB3C5651896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{11EE884C-F399-9F46-A5ED-E6B519B3281B}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{7894EA0F-3342-2140-B87D-CBB3C5651896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08C6FDE6-E52D-FB49-A6A3-3A37E13182DB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26760" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -416,7 +418,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -439,7 +441,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>4</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -453,7 +455,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D5" s="1">
         <f>D3*(C6+C8)/C10</f>
-        <v>1.8326309452137266</v>
+        <v>1.5119205298013243</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -465,7 +467,7 @@
       </c>
       <c r="D6" s="1">
         <f>D5-D7</f>
-        <v>2.6490066225165476E-2</v>
+        <v>2.1854304635761324E-2</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -474,7 +476,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" s="1">
         <f>D3*(C8)/C10</f>
-        <v>1.8061408789885611</v>
+        <v>1.490066225165563</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Implement Core_Mem_Bit_Read and testing sense pulse width
</commit_message>
<xml_diff>
--- a/Electronic Design/core flip sense voltage threshold.xlsx
+++ b/Electronic Design/core flip sense voltage threshold.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{7894EA0F-3342-2140-B87D-CBB3C5651896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08C6FDE6-E52D-FB49-A6A3-3A37E13182DB}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{7894EA0F-3342-2140-B87D-CBB3C5651896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DC52F918-B4D9-B040-AB89-3FE08D2E5E45}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26760" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="23060" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>V+</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>&lt;- Delta V</t>
+  </si>
+  <si>
+    <t>Jussi Kilpelainen's shield design values</t>
+  </si>
+  <si>
+    <t>Rolfe Bozier's shield design values</t>
+  </si>
+  <si>
+    <t>Andy's  design values</t>
   </si>
 </sst>
 </file>
@@ -78,12 +87,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,9 +113,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,96 +432,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61078911-D8CC-2A48-8A33-C4BCF8F618F6}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="E4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C5" s="2"/>
+      <c r="D5" s="3">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="E5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="L5" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="O5" s="1">
+        <v>5</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="3">
+        <v>5</v>
+      </c>
+      <c r="U5" s="2"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C6" s="2">
         <v>1800</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D5" s="1">
-        <f>D3*(C6+C8)/C10</f>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1800</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="R6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" s="2">
+        <v>3300</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3">
+        <f>D5*($C8+$C10)/$C12</f>
         <v>1.5119205298013243</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="E7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3">
+        <f>I5*($H8+$H10)/$H12</f>
+        <v>1.5073877353935294</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="L7" s="1">
+        <f>L5*($C8+$C10)/$C12</f>
+        <v>2.0617098133654426</v>
+      </c>
+      <c r="O7" s="1">
+        <f>O5*($C8+$C10)/$C12</f>
+        <v>2.2907886815171583</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3">
+        <f>T5*($S8+$S10)/$S12</f>
+        <v>1.6463414634146341</v>
+      </c>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C8" s="2">
         <v>22</v>
       </c>
-      <c r="D6" s="1">
-        <f>D5-D7</f>
+      <c r="D8" s="3">
+        <f>D7-D9</f>
         <v>2.1854304635761324E-2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D7" s="1">
-        <f>D3*(C8)/C10</f>
+      <c r="G8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
+        <f>2*6.8</f>
+        <v>13.6</v>
+      </c>
+      <c r="I8" s="3">
+        <f>I7-I9</f>
+        <v>1.354418155480408E-2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="1">
+        <f>L7-L9</f>
+        <v>2.9801324503311299E-2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" s="1">
+        <f>O7-O9</f>
+        <v>3.3112582781456901E-2</v>
+      </c>
+      <c r="P8" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="2">
+        <v>20</v>
+      </c>
+      <c r="T8" s="3">
+        <f>T7-T9</f>
+        <v>2.0325203252032464E-2</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3">
+        <f>D5*($C10)/$C12</f>
         <v>1.490066225165563</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="E9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3">
+        <f>I5*($H10)/$H12</f>
+        <v>1.4938435538387254</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="L9" s="1">
+        <f>L5*($C10)/$C12</f>
+        <v>2.0319084888621313</v>
+      </c>
+      <c r="O9" s="1">
+        <f>O5*($C10)/$C12</f>
+        <v>2.2576760987357014</v>
+      </c>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="3">
+        <f>T5*($S10)/$S12</f>
+        <v>1.6260162601626016</v>
+      </c>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C10" s="2">
         <v>1500</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1500</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="2"/>
+      <c r="L10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="R10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10" s="2">
+        <v>1600</v>
+      </c>
+      <c r="T10" s="3"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="E11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="3">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <f>SUM(C4:C8)</f>
+      <c r="C12" s="2">
+        <f>SUM(C6:C10)</f>
         <v>3322</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <f>SUM(H6:H10)</f>
+        <v>3313.6</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="2"/>
+      <c r="L12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="R12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S12" s="2">
+        <f>SUM(S6:S10)</f>
+        <v>4920</v>
+      </c>
+      <c r="T12" s="3"/>
+      <c r="U12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sense resistor changes make it more reliable!
</commit_message>
<xml_diff>
--- a/Electronic Design/core flip sense voltage threshold.xlsx
+++ b/Electronic Design/core flip sense voltage threshold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{7894EA0F-3342-2140-B87D-CBB3C5651896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DC52F918-B4D9-B040-AB89-3FE08D2E5E45}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{7894EA0F-3342-2140-B87D-CBB3C5651896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87808549-E18C-E44F-BECA-93238981EEE7}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23060" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +97,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,11 +119,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +443,7 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -452,9 +460,12 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="R3" s="2" t="s">
         <v>11</v>
       </c>
@@ -471,14 +482,14 @@
         <v>7</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="4"/>
       <c r="L4" t="s">
         <v>7</v>
       </c>
@@ -503,14 +514,14 @@
         <v>3.3</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3">
+      <c r="H5" s="4"/>
+      <c r="I5" s="5">
         <v>3.3</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="4"/>
       <c r="L5" s="1">
         <v>4.5</v>
       </c>
@@ -535,14 +546,14 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="4">
         <v>1800</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
       <c r="R6" s="2" t="s">
         <v>1</v>
       </c>
@@ -560,13 +571,13 @@
         <v>1.5119205298013243</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5">
         <f>I5*($H8+$H10)/$H12</f>
-        <v>1.5073877353935294</v>
-      </c>
-      <c r="J7" s="2"/>
+        <v>1.5059800664451828</v>
+      </c>
+      <c r="J7" s="4"/>
       <c r="L7" s="1">
         <f>L5*($C8+$C10)/$C12</f>
         <v>2.0617098133654426</v>
@@ -597,18 +608,17 @@
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="2">
-        <f>2*6.8</f>
-        <v>13.6</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="H8" s="4">
+        <v>11</v>
+      </c>
+      <c r="I8" s="5">
         <f>I7-I9</f>
-        <v>1.354418155480408E-2</v>
-      </c>
-      <c r="J8" s="2" t="s">
+        <v>1.09634551495017E-2</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L8" s="1">
@@ -647,13 +657,13 @@
         <v>1.490066225165563</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5">
         <f>I5*($H10)/$H12</f>
-        <v>1.4938435538387254</v>
-      </c>
-      <c r="J9" s="2"/>
+        <v>1.4950166112956811</v>
+      </c>
+      <c r="J9" s="4"/>
       <c r="L9" s="1">
         <f>L5*($C10)/$C12</f>
         <v>2.0319084888621313</v>
@@ -679,14 +689,14 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="4">
         <v>1500</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="2"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="4"/>
       <c r="L10" s="1"/>
       <c r="O10" s="1"/>
       <c r="R10" s="2" t="s">
@@ -707,14 +717,14 @@
         <v>0</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3">
+      <c r="H11" s="4"/>
+      <c r="I11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="4"/>
       <c r="L11" s="1">
         <v>0</v>
       </c>
@@ -740,15 +750,15 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="2"/>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="4">
         <f>SUM(H6:H10)</f>
-        <v>3313.6</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="2"/>
+        <v>3311</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4"/>
       <c r="L12" s="1"/>
       <c r="O12" s="1"/>
       <c r="R12" s="2" t="s">

</xml_diff>

<commit_message>
Updated flip sense resistors 22 to 11 Ohm
</commit_message>
<xml_diff>
--- a/Electronic Design/core flip sense voltage threshold.xlsx
+++ b/Electronic Design/core flip sense voltage threshold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{7894EA0F-3342-2140-B87D-CBB3C5651896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87808549-E18C-E44F-BECA-93238981EEE7}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{7894EA0F-3342-2140-B87D-CBB3C5651896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9FA610F1-C02D-9043-A921-84E46755144D}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="23060" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,7 +102,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,7 +443,7 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>